<commit_message>
Update all race results.
</commit_message>
<xml_diff>
--- a/docs/RESULTS 1000km.xlsx
+++ b/docs/RESULTS 1000km.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="9390"/>
@@ -23,12 +23,6 @@
     <t>RESULT</t>
   </si>
   <si>
-    <t>SURNAME</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
     <t>M/F</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
   </si>
   <si>
     <t>1000 klm</t>
-  </si>
-  <si>
-    <t>1000klm.  RACE RESULTS</t>
   </si>
   <si>
     <t xml:space="preserve">MARIFOGLOU  </t>
@@ -1036,12 +1027,21 @@
   </si>
   <si>
     <t>……………..</t>
+  </si>
+  <si>
+    <t>NAME                (SURNAME)</t>
+  </si>
+  <si>
+    <t>FIRST    NAME</t>
+  </si>
+  <si>
+    <t>1000km  RACE RESULTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1208,7 +1208,7 @@
       <charset val="161"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1230,6 +1230,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1274,7 +1280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1346,21 +1352,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1376,7 +1397,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1418,7 +1439,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1451,9 +1472,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1486,6 +1524,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1664,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1730,7 @@
     <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" customWidth="1"/>
     <col min="9" max="9" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -1686,349 +1741,350 @@
     <col min="14" max="14" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G2" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="29" t="s">
-        <v>32</v>
+    <row r="3" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="27" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:14" s="35" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="28" t="s">
-        <v>29</v>
-      </c>
+      <c r="N4" s="34"/>
     </row>
-    <row r="5" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>1</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>13</v>
+        <v>48</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>52</v>
+      <c r="B6" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="L6" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <v>3</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>53</v>
+      <c r="B7" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="F7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="J7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="M7" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <v>4</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>54</v>
+      <c r="B8" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>39</v>
-      </c>
       <c r="H8" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <v>5</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>55</v>
+      <c r="B9" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="H9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="J9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
         <v>6</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>56</v>
+      <c r="B10" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="H10" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <v>7</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="G11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>48</v>
-      </c>
       <c r="H11" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" s="30" t="s">
-        <v>57</v>
+        <v>25</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="26"/>

</xml_diff>